<commit_message>
Mod : edit Text En to Kr
</commit_message>
<xml_diff>
--- a/NaverPowerLinkRanking/MultiSearchTestSample/Test Sample4.xlsx
+++ b/NaverPowerLinkRanking/MultiSearchTestSample/Test Sample4.xlsx
@@ -27,9 +27,6 @@
     <t>KEYWORD</t>
   </si>
   <si>
-    <t>http://lstorymall.co.kr</t>
-  </si>
-  <si>
     <t>LED공장등</t>
   </si>
   <si>
@@ -121,13 +118,17 @@
   </si>
   <si>
     <t>엘이디공장등</t>
+  </si>
+  <si>
+    <t>http://lstorymall.co.kr/</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,6 +283,15 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
@@ -585,7 +595,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -712,13 +722,19 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - 강조색1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - 강조색2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - 강조색3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -761,6 +777,7 @@
     <cellStyle name="좋음" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="출력" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="하이퍼링크" xfId="42" builtinId="8"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1071,6 +1088,9 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1081,255 +1101,256 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>2</v>
-      </c>
-      <c r="B24" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>2</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>2</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>2</v>
-      </c>
-      <c r="B27" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>2</v>
-      </c>
-      <c r="B28" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>2</v>
-      </c>
-      <c r="B29" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>2</v>
-      </c>
-      <c r="B30" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>2</v>
-      </c>
-      <c r="B31" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>2</v>
-      </c>
-      <c r="B32" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add & mod test samples
</commit_message>
<xml_diff>
--- a/NaverPowerLinkRanking/MultiSearchTestSample/Test Sample4.xlsx
+++ b/NaverPowerLinkRanking/MultiSearchTestSample/Test Sample4.xlsx
@@ -27,6 +27,9 @@
     <t>KEYWORD</t>
   </si>
   <si>
+    <t>http://lstorymall.co.kr</t>
+  </si>
+  <si>
     <t>LED공장등</t>
   </si>
   <si>
@@ -118,17 +121,13 @@
   </si>
   <si>
     <t>엘이디공장등</t>
-  </si>
-  <si>
-    <t>http://lstorymall.co.kr/</t>
-    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,15 +282,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
@@ -595,7 +585,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -722,19 +712,13 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="42">
     <cellStyle name="20% - 강조색1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - 강조색2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - 강조색3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -777,7 +761,6 @@
     <cellStyle name="좋음" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="출력" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="하이퍼링크" xfId="42" builtinId="8"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1088,9 +1071,6 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1101,256 +1081,255 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" t="s">
         <v>33</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B31" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>